<commit_message>
updates and clean up of data
</commit_message>
<xml_diff>
--- a/data/final/fertility_art_cycles.xlsx
+++ b/data/final/fertility_art_cycles.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t xml:space="preserve">Cycle type</t>
   </si>
@@ -54,21 +54,6 @@
   </si>
   <si>
     <t xml:space="preserve">Embryo recipient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Occyte donation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Embryo donation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surrogacy gestational carrier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surrogacy commissioning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lab-only</t>
   </si>
   <si>
     <t xml:space="preserve">Total</t>
@@ -122,6 +107,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -143,12 +129,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -193,12 +181,8 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -231,13 +215,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.57"/>
@@ -255,273 +239,200 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3" t="n">
+      <c r="B2" s="2" t="n">
         <v>65414</v>
       </c>
-      <c r="C2" s="3" t="n">
+      <c r="C2" s="2" t="n">
         <v>22685</v>
       </c>
-      <c r="D2" s="3" t="n">
+      <c r="D2" s="2" t="n">
         <v>26107</v>
       </c>
-      <c r="E2" s="3" t="n">
+      <c r="E2" s="2" t="n">
         <v>8496</v>
       </c>
-      <c r="F2" s="3" t="n">
+      <c r="F2" s="2" t="n">
         <v>6607</v>
       </c>
-      <c r="G2" s="3" t="n">
+      <c r="G2" s="2" t="n">
         <v>6822</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="3" t="n">
+      <c r="B3" s="2" t="n">
         <v>39503</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3" t="n">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="n">
         <v>38731</v>
       </c>
-      <c r="E3" s="3" t="n">
+      <c r="E3" s="2" t="n">
         <v>15252</v>
       </c>
-      <c r="F3" s="3" t="n">
+      <c r="F3" s="2" t="n">
         <v>12213</v>
       </c>
-      <c r="G3" s="3" t="n">
+      <c r="G3" s="2" t="n">
         <v>12566</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="3" t="n">
+      <c r="B4" s="2" t="n">
         <v>2360</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3" t="n">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="n">
         <v>2077</v>
       </c>
-      <c r="E4" s="3" t="n">
+      <c r="E4" s="2" t="n">
         <v>763</v>
       </c>
-      <c r="F4" s="3" t="n">
+      <c r="F4" s="2" t="n">
         <v>600</v>
       </c>
-      <c r="G4" s="3" t="n">
+      <c r="G4" s="2" t="n">
         <v>622</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="3" t="n">
+      <c r="B5" s="2" t="n">
         <v>996</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3" t="n">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="n">
         <v>979</v>
       </c>
-      <c r="E5" s="3" t="n">
+      <c r="E5" s="2" t="n">
         <v>394</v>
       </c>
-      <c r="F5" s="3" t="n">
+      <c r="F5" s="2" t="n">
         <v>322</v>
       </c>
-      <c r="G5" s="3" t="n">
+      <c r="G5" s="2" t="n">
         <v>330</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="3" t="n">
-        <v>1187</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="B6" s="1" t="n">
+        <f aca="false">SUM(B2:B5)</f>
+        <v>108273</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <f aca="false">SUM(C2:C5)</f>
+        <v>22685</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <f aca="false">SUM(D2:D5)</f>
+        <v>67894</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <f aca="false">SUM(E2:E5)</f>
+        <v>24905</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <f aca="false">SUM(F2:F5)</f>
+        <v>19742</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <f aca="false">SUM(G2:G5)</f>
+        <v>20340</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="3" t="n">
-        <v>70</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="3" t="n">
-        <v>280</v>
-      </c>
-      <c r="C8" s="3"/>
+        <f aca="false">SUM(B2:B3)</f>
+        <v>104917</v>
+      </c>
+      <c r="C8" s="3" t="n">
+        <f aca="false">SUM(C2:C3)</f>
+        <v>22685</v>
+      </c>
       <c r="D8" s="3" t="n">
-        <v>274</v>
+        <f aca="false">SUM(D2:D3)</f>
+        <v>64838</v>
       </c>
       <c r="E8" s="3" t="n">
-        <v>123</v>
+        <f aca="false">SUM(E2:E3)</f>
+        <v>23748</v>
       </c>
       <c r="F8" s="3" t="n">
-        <v>100</v>
+        <f aca="false">SUM(F2:F3)</f>
+        <v>18820</v>
       </c>
       <c r="G8" s="3" t="n">
-        <v>100</v>
+        <f aca="false">SUM(G2:G3)</f>
+        <v>19388</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="3" t="n">
-        <v>120</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="3" t="n">
-        <v>1323</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="2" t="n">
-        <f aca="false">SUM(B2:B10)</f>
-        <v>111253</v>
-      </c>
-      <c r="C11" s="2" t="n">
-        <f aca="false">SUM(C2:C10)</f>
-        <v>22685</v>
-      </c>
-      <c r="D11" s="2" t="n">
-        <f aca="false">SUM(D2:D10)</f>
-        <v>68168</v>
-      </c>
-      <c r="E11" s="2" t="n">
-        <f aca="false">SUM(E2:E10)</f>
-        <v>25028</v>
-      </c>
-      <c r="F11" s="2" t="n">
-        <f aca="false">SUM(F2:F10)</f>
-        <v>19842</v>
-      </c>
-      <c r="G11" s="2" t="n">
-        <f aca="false">SUM(G2:G10)</f>
-        <v>20440</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="4" t="n">
-        <f aca="false">SUM(B2:B3)</f>
-        <v>104917</v>
-      </c>
-      <c r="C13" s="4" t="n">
-        <f aca="false">SUM(C2:C3)</f>
-        <v>22685</v>
-      </c>
-      <c r="D13" s="4" t="n">
-        <f aca="false">SUM(D2:D3)</f>
-        <v>64838</v>
-      </c>
-      <c r="E13" s="4" t="n">
-        <f aca="false">SUM(E2:E3)</f>
-        <v>23748</v>
-      </c>
-      <c r="F13" s="4" t="n">
-        <f aca="false">SUM(F2:F3)</f>
-        <v>18820</v>
-      </c>
-      <c r="G13" s="4" t="n">
-        <f aca="false">SUM(G2:G3)</f>
-        <v>19388</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="4" t="n">
         <f aca="false">SUM(B2:B5)</f>
         <v>108273</v>
       </c>
-      <c r="C14" s="4" t="n">
+      <c r="C9" s="3" t="n">
         <f aca="false">SUM(C2:C5)</f>
         <v>22685</v>
       </c>
-      <c r="D14" s="4" t="n">
+      <c r="D9" s="3" t="n">
         <f aca="false">SUM(D2:D5)</f>
         <v>67894</v>
       </c>
-      <c r="E14" s="4" t="n">
+      <c r="E9" s="3" t="n">
         <f aca="false">SUM(E2:E5)</f>
         <v>24905</v>
       </c>
-      <c r="F14" s="4" t="n">
+      <c r="F9" s="3" t="n">
         <f aca="false">SUM(F2:F5)</f>
         <v>19742</v>
       </c>
-      <c r="G14" s="4" t="n">
+      <c r="G9" s="3" t="n">
         <f aca="false">SUM(G2:G5)</f>
         <v>20340</v>
       </c>
@@ -548,34 +459,34 @@
       <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.46"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>3</v>
@@ -592,10 +503,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>22685</v>
@@ -609,10 +520,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>17694</v>
@@ -629,7 +540,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>24905</v>
@@ -643,10 +554,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>19742</v>
@@ -660,7 +571,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>6</v>

</xml_diff>